<commit_message>
updated concept system output based on revisions
</commit_message>
<xml_diff>
--- a/Output_Folders/concept_system_output/Full_results_all_models_EXT.xlsx
+++ b/Output_Folders/concept_system_output/Full_results_all_models_EXT.xlsx
@@ -1,49 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MaylaB/Dropbox/Documents/0_Thesis_stuff-Larry_Sonia/Negacy_seq_2_seq_NER_model/ConceptRecognition/concept_system_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3102FA4F-B900-6D4C-B156-DD471157E60A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E986C4-744E-3748-8BB6-4BE34DA99D0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16620" activeTab="1" xr2:uid="{A11FB7C2-6A24-434A-8059-7C581917F3EC}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16620" xr2:uid="{A11FB7C2-6A24-434A-8059-7C581917F3EC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Best Results - SO FAR" sheetId="5" r:id="rId1"/>
-    <sheet name="EXT-discontinuous spans" sheetId="19" r:id="rId2"/>
-    <sheet name="CHEBI_EXT" sheetId="9" r:id="rId3"/>
-    <sheet name="CL_EXT" sheetId="10" r:id="rId4"/>
-    <sheet name="GO_BP_EXT" sheetId="11" r:id="rId5"/>
-    <sheet name="GO_CC_EXT" sheetId="12" r:id="rId6"/>
-    <sheet name="GO_MF_EXT" sheetId="13" r:id="rId7"/>
-    <sheet name="MOP_EXT" sheetId="14" r:id="rId8"/>
-    <sheet name="NCBITaxon_EXT" sheetId="15" r:id="rId9"/>
-    <sheet name="PR_EXT" sheetId="16" r:id="rId10"/>
-    <sheet name="SO_EXT" sheetId="17" r:id="rId11"/>
-    <sheet name="UBERON_EXT" sheetId="18" r:id="rId12"/>
-    <sheet name="CRF" sheetId="1" r:id="rId13"/>
-    <sheet name="LSTM" sheetId="2" r:id="rId14"/>
-    <sheet name="LSTM-CRF" sheetId="3" r:id="rId15"/>
-    <sheet name="CHAR_EMBEDDING LSTM" sheetId="4" r:id="rId16"/>
-    <sheet name="LSTM-ELMO" sheetId="7" r:id="rId17"/>
-    <sheet name="BIOBERT" sheetId="8" r:id="rId18"/>
-    <sheet name="OGER" sheetId="6" r:id="rId19"/>
+    <sheet name="EXT - updated results" sheetId="20" r:id="rId1"/>
+    <sheet name="Best Results - SO FAR" sheetId="5" r:id="rId2"/>
+    <sheet name="EXT-discontinuous spans" sheetId="19" r:id="rId3"/>
+    <sheet name="CHEBI_EXT" sheetId="9" r:id="rId4"/>
+    <sheet name="CL_EXT" sheetId="10" r:id="rId5"/>
+    <sheet name="GO_BP_EXT" sheetId="11" r:id="rId6"/>
+    <sheet name="GO_CC_EXT" sheetId="12" r:id="rId7"/>
+    <sheet name="GO_MF_EXT" sheetId="13" r:id="rId8"/>
+    <sheet name="MOP_EXT" sheetId="14" r:id="rId9"/>
+    <sheet name="NCBITaxon_EXT" sheetId="15" r:id="rId10"/>
+    <sheet name="PR_EXT" sheetId="16" r:id="rId11"/>
+    <sheet name="SO_EXT" sheetId="17" r:id="rId12"/>
+    <sheet name="UBERON_EXT" sheetId="18" r:id="rId13"/>
+    <sheet name="CRF" sheetId="1" r:id="rId14"/>
+    <sheet name="LSTM" sheetId="2" r:id="rId15"/>
+    <sheet name="LSTM-CRF" sheetId="3" r:id="rId16"/>
+    <sheet name="CHAR_EMBEDDING LSTM" sheetId="4" r:id="rId17"/>
+    <sheet name="LSTM-ELMO" sheetId="7" r:id="rId18"/>
+    <sheet name="BIOBERT" sheetId="8" r:id="rId19"/>
+    <sheet name="OGER" sheetId="6" r:id="rId20"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CHEBI_EXT!$A$1:$E$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CL_EXT!$A$1:$E$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">GO_BP_EXT!$A$1:$E$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">GO_CC_EXT!$A$1:$E$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">GO_MF_EXT!$A$1:$E$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">MOP_EXT!$A$1:$E$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">NCBITaxon_EXT!$A$1:$E$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">PR_EXT!$A$1:$E$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">SO_EXT!$A$1:$E$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">UBERON_EXT!$A$1:$E$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CHEBI_EXT!$A$1:$E$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">CL_EXT!$A$1:$E$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">GO_BP_EXT!$A$1:$E$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">GO_CC_EXT!$A$1:$E$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">GO_MF_EXT!$A$1:$E$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">MOP_EXT!$A$1:$E$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">NCBITaxon_EXT!$A$1:$E$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">PR_EXT!$A$1:$E$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">SO_EXT!$A$1:$E$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">UBERON_EXT!$A$1:$E$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="47">
   <si>
     <t>ONTOLOGY</t>
   </si>
@@ -210,7 +211,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -222,6 +223,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -280,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -288,6 +296,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,339 +611,166 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDEF1579-F43D-B24D-9E1F-9AC07B95705A}">
-  <dimension ref="A1:M11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3132355-E209-7D45-A1D6-FA68B8CADFFB}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="4">
-        <v>0.31190000000000001</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.77700000000000002</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0.74550000000000005</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0.76090000000000002</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="6" t="s">
+      <c r="D1" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="1">
+      <c r="B2">
+        <v>0.78910000000000002</v>
+      </c>
+      <c r="C2">
+        <v>0.80389999999999995</v>
+      </c>
+      <c r="D2" s="8">
         <v>0.82089999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.36359999999999998</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.71360000000000001</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.7238</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.71870000000000001</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" s="6" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="1">
+      <c r="B3">
+        <v>0.73809999999999998</v>
+      </c>
+      <c r="C3">
+        <v>0.74909999999999999</v>
+      </c>
+      <c r="D3" s="8">
         <v>0.74839999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.33129999999999998</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.7238</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.7268</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.72529999999999994</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="6" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="1">
+      <c r="B4">
+        <v>0.72789999999999999</v>
+      </c>
+      <c r="C4">
+        <v>0.73529999999999995</v>
+      </c>
+      <c r="D4" s="8">
         <v>0.81379999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.16880000000000001</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.89329999999999998</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.88239999999999996</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.88780000000000003</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" s="6" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="1">
+      <c r="B5">
+        <v>0.87380000000000002</v>
+      </c>
+      <c r="C5">
+        <v>0.89829999999999999</v>
+      </c>
+      <c r="D5" s="8">
         <v>0.89359999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.47889999999999999</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.67910000000000004</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.57440000000000002</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.62239999999999995</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="6" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="1">
+      <c r="B6">
+        <v>0.64129999999999998</v>
+      </c>
+      <c r="C6">
+        <v>0.62549999999999994</v>
+      </c>
+      <c r="D6" s="8">
         <v>0.74380000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.26340000000000002</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.81469999999999998</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.88080000000000003</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.84640000000000004</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" s="6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M7" s="1">
+      <c r="B7">
+        <v>0.8</v>
+      </c>
+      <c r="C7">
+        <v>0.86509999999999998</v>
+      </c>
+      <c r="D7" s="8">
         <v>0.84370000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="4">
-        <v>4.4299999999999999E-2</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.96919999999999995</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.96530000000000005</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0.96730000000000005</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8" s="6" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="1">
+      <c r="B8">
+        <v>0.871</v>
+      </c>
+      <c r="C8">
+        <v>0.86240000000000006</v>
+      </c>
+      <c r="D8" s="8">
         <v>0.97219999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.5484</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.5464</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.6018</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.57269999999999999</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L9" s="6" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="M9" s="1">
+      <c r="B9">
+        <v>0.43969999999999998</v>
+      </c>
+      <c r="C9">
+        <v>0.51880000000000004</v>
+      </c>
+      <c r="D9" s="8">
         <v>0.80110000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0.27479999999999999</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.79310000000000003</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0.74860000000000004</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0.7702</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="6" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="M10" s="1">
+      <c r="B10">
+        <v>0.76819999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.78290000000000004</v>
+      </c>
+      <c r="D10" s="8">
         <v>0.91869999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0.33289999999999997</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.74939999999999996</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0.71940000000000004</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0.73409999999999997</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L11" s="6" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="M11" s="1">
+      <c r="B11">
+        <v>0.75580000000000003</v>
+      </c>
+      <c r="C11">
+        <v>0.77110000000000001</v>
+      </c>
+      <c r="D11" s="8">
         <v>0.77139999999999997</v>
       </c>
     </row>
@@ -943,6 +780,190 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A89592-5FFC-BF47-85CA-8131A731E917}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="5">
+        <f>OGER!B$8</f>
+        <v>0.97219999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1">
+        <f>BIOBERT!B$8</f>
+        <v>4.4299999999999999E-2</v>
+      </c>
+      <c r="C3" s="1">
+        <f>BIOBERT!C$8</f>
+        <v>0.96919999999999995</v>
+      </c>
+      <c r="D3" s="1">
+        <f>BIOBERT!D$8</f>
+        <v>0.96530000000000005</v>
+      </c>
+      <c r="E3" s="1">
+        <f>BIOBERT!E$8</f>
+        <v>0.96730000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1">
+        <f>CRF!B$8</f>
+        <v>0.9667</v>
+      </c>
+      <c r="C4" s="1">
+        <f>CRF!C$8</f>
+        <v>5.9700000000000003E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <f>CRF!D$8</f>
+        <v>0.98140000000000005</v>
+      </c>
+      <c r="E4" s="1">
+        <f>CRF!E$8</f>
+        <v>0.95240000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1">
+        <f>'CHAR_EMBEDDING LSTM'!B$8</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <f>'CHAR_EMBEDDING LSTM'!C$8</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <f>'CHAR_EMBEDDING LSTM'!D$8</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <f>'CHAR_EMBEDDING LSTM'!E$8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1">
+        <f>LSTM!B$8</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <f>LSTM!C$8</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <f>LSTM!D$8</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <f>LSTM!E$8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1">
+        <f>'LSTM-CRF'!B$8</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <f>'LSTM-CRF'!C$8</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <f>'LSTM-CRF'!D$8</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <f>'LSTM-CRF'!E$8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1">
+        <f>'LSTM-ELMO'!B$8</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <f>'LSTM-ELMO'!C$8</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <f>'LSTM-ELMO'!D$8</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <f>'LSTM-ELMO'!E$8</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E8" xr:uid="{563C96C5-AA5E-CF47-BBFA-B0EE84DEB98F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E8">
+      <sortCondition descending="1" ref="E1:E8"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE95C83F-D092-0640-B08C-61E5B7ADCAF8}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -1126,7 +1147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8109C2D-4BA9-EA48-88CC-B36539869B65}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -1310,7 +1331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA28A23-0A6E-3442-AE03-4EEFF6E90EE5}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -1494,7 +1515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBD22BE-0061-D149-BD9B-43F0D337174F}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -1696,7 +1717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC048289-4AEB-6649-B213-17B0CBCAAA1D}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -1818,7 +1839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03264D92-EE09-B242-A352-B8E655B36B5E}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -1940,7 +1961,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B909ED-91EF-AC45-8515-C5B0E377DF1E}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -2062,7 +2083,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6ABD706-3641-A64B-97F3-2073EB88F734}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -2184,7 +2205,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02C32E2-8B4A-0B49-9B00-D874283FDC73}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -2389,7 +2410,349 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDEF1579-F43D-B24D-9E1F-9AC07B95705A}">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.31190000000000001</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.74550000000000005</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.76090000000000002</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.82089999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.36359999999999998</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.71360000000000001</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.7238</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.71870000000000001</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.74839999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.33129999999999998</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.7238</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.7268</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.72529999999999994</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.81379999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.16880000000000001</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.89329999999999998</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.88239999999999996</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.88780000000000003</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.89359999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.47889999999999999</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.67910000000000004</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.57440000000000002</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.62239999999999995</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.74380000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.26340000000000002</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.81469999999999998</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.88080000000000003</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.84640000000000004</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.84370000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4">
+        <v>4.4299999999999999E-2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.96919999999999995</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.96530000000000005</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.96730000000000005</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.97219999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.5484</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.5464</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.6018</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.57269999999999999</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0.80110000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.27479999999999999</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.79310000000000003</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.74860000000000004</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.7702</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0.91869999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.33289999999999997</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.74939999999999996</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.71940000000000004</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.73409999999999997</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0.77139999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FA76E5-009A-2646-A388-B08C38139CF7}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -2496,11 +2859,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F3B1B7-898E-5643-8B38-BD905B3272E3}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2661,7 +3024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EA9396-3A02-6F42-A11C-CA43A954929A}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -2845,7 +3208,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EB0735-9B05-C64B-8EB9-9728F5E9B082}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -3029,7 +3392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03913A76-6295-E14A-8923-04A39550C8F0}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -3213,7 +3576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61D3962-240C-2A46-B335-8F611C7BC358}">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -3400,7 +3763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBAEB33-7ED7-C84D-88F7-BF427E5EF640}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -3584,7 +3947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98AB7D1C-EAD7-594B-847D-E7AE6EB73DF3}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -3766,188 +4129,4 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A89592-5FFC-BF47-85CA-8131A731E917}">
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="5">
-        <f>OGER!B$8</f>
-        <v>0.97219999999999995</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1">
-        <f>BIOBERT!B$8</f>
-        <v>4.4299999999999999E-2</v>
-      </c>
-      <c r="C3" s="1">
-        <f>BIOBERT!C$8</f>
-        <v>0.96919999999999995</v>
-      </c>
-      <c r="D3" s="1">
-        <f>BIOBERT!D$8</f>
-        <v>0.96530000000000005</v>
-      </c>
-      <c r="E3" s="1">
-        <f>BIOBERT!E$8</f>
-        <v>0.96730000000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1">
-        <f>CRF!B$8</f>
-        <v>0.9667</v>
-      </c>
-      <c r="C4" s="1">
-        <f>CRF!C$8</f>
-        <v>5.9700000000000003E-2</v>
-      </c>
-      <c r="D4" s="1">
-        <f>CRF!D$8</f>
-        <v>0.98140000000000005</v>
-      </c>
-      <c r="E4" s="1">
-        <f>CRF!E$8</f>
-        <v>0.95240000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="1">
-        <f>'CHAR_EMBEDDING LSTM'!B$8</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <f>'CHAR_EMBEDDING LSTM'!C$8</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <f>'CHAR_EMBEDDING LSTM'!D$8</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <f>'CHAR_EMBEDDING LSTM'!E$8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1">
-        <f>LSTM!B$8</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <f>LSTM!C$8</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <f>LSTM!D$8</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <f>LSTM!E$8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="1">
-        <f>'LSTM-CRF'!B$8</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <f>'LSTM-CRF'!C$8</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <f>'LSTM-CRF'!D$8</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <f>'LSTM-CRF'!E$8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="1">
-        <f>'LSTM-ELMO'!B$8</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <f>'LSTM-ELMO'!C$8</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <f>'LSTM-ELMO'!D$8</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <f>'LSTM-ELMO'!E$8</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:E8" xr:uid="{563C96C5-AA5E-CF47-BBFA-B0EE84DEB98F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E8">
-      <sortCondition descending="1" ref="E1:E8"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>